<commit_message>
Formato de seguimiento 17/03/2015
</commit_message>
<xml_diff>
--- a/seguimiento/Grado04.xlsx
+++ b/seguimiento/Grado04.xlsx
@@ -68,49 +68,7 @@
     <t>Matemáticas</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>12/03/2015:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Se revisan y quedan aprobados los gráficos presentados por la documentadora, para el manuscrito (MA_04_01_CO) y las fotografías de los recursos MA_04_01_REC100, REC50, REC40, REC70.
-Hace falta hasta la fecha (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>15/03/2015</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>), que la documentadora gráfica incluya un PDF con las ilustraciones solicitadas en los recursos: REC80, REC90, REC170, REC190, REC210, REC220.</t>
-    </r>
+    <t>Queda aprobado material gráfico.</t>
   </si>
 </sst>
 </file>
@@ -979,7 +937,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="270.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29">
         <v>1</v>
       </c>
@@ -992,7 +950,9 @@
       <c r="D6" s="5">
         <v>42070</v>
       </c>
-      <c r="E6" s="5"/>
+      <c r="E6" s="5">
+        <v>42080</v>
+      </c>
       <c r="F6" s="6" t="s">
         <v>14</v>
       </c>

</xml_diff>